<commit_message>
add chocolate rating table in resources
</commit_message>
<xml_diff>
--- a/Work allocation.xlsx
+++ b/Work allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\UWA Data Bootcamp\13. ETL-Project\ETL_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BFCE12D-5317-476D-BD43-DCB6E4178C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E29779C-156D-4845-8A28-4A9EBB865BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{20BA0EC7-7DF8-4BE8-AAD7-E60F10A95A69}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>Output</t>
   </si>
@@ -97,16 +97,46 @@
   </si>
   <si>
     <t>Melissa</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>Melissa/Kevin</t>
+  </si>
+  <si>
+    <t>Combining SQL schema</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>supply_utilisation csv</t>
+  </si>
+  <si>
+    <t>Chocolate_rating csv</t>
+  </si>
+  <si>
+    <t>Cocoa  Prices - Daily csv</t>
+  </si>
+  <si>
+    <t>Cocoa Prices - Monthly average csv</t>
+  </si>
+  <si>
+    <t>Create aggregate on min &amp; max based on year</t>
+  </si>
+  <si>
+    <t>Crop livestock production csv</t>
+  </si>
+  <si>
+    <t>detailed trade matrix csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,13 +146,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -144,7 +167,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -167,12 +190,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -182,10 +230,26 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -498,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F689A68A-4E99-4027-9313-5972ED85C8C1}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +610,9 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -572,82 +638,174 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
+      <c r="A7" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="9" t="s">
+        <v>5</v>
+      </c>
       <c r="E9" s="4"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="4"/>
       <c r="F10" s="2"/>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="2"/>
+    </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F10" xr:uid="{F689A68A-4E99-4027-9313-5972ED85C8C1}"/>
+  <autoFilter ref="A1:F11" xr:uid="{F689A68A-4E99-4027-9313-5972ED85C8C1}"/>
+  <mergeCells count="3">
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
upload new work allocation
</commit_message>
<xml_diff>
--- a/Work allocation.xlsx
+++ b/Work allocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\UWA Data Bootcamp\13. ETL-Project\ETL_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E29779C-156D-4845-8A28-4A9EBB865BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF67C360-32F4-46D2-B3A8-DAA978836814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{20BA0EC7-7DF8-4BE8-AAD7-E60F10A95A69}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>Output</t>
   </si>
@@ -84,18 +84,9 @@
     <t xml:space="preserve">Create tables &amp; schema in SQL </t>
   </si>
   <si>
-    <t>Look at chocolate rating table</t>
-  </si>
-  <si>
-    <t>Cocoa Pricing table</t>
-  </si>
-  <si>
     <t>Thursday/Monday</t>
   </si>
   <si>
-    <t>FAO Tables (6 tables) to be allocated amongst all 4 team members</t>
-  </si>
-  <si>
     <t>Melissa</t>
   </si>
   <si>
@@ -129,7 +120,16 @@
     <t>Crop livestock production csv</t>
   </si>
   <si>
-    <t>detailed trade matrix csv</t>
+    <t>Tables:</t>
+  </si>
+  <si>
+    <t>Detailed trade matrix csv</t>
+  </si>
+  <si>
+    <t>Production_indices</t>
+  </si>
+  <si>
+    <t>Value Agriculture</t>
   </si>
 </sst>
 </file>
@@ -153,7 +153,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,8 +166,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -216,11 +222,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -236,17 +290,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F689A68A-4E99-4027-9313-5972ED85C8C1}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C9" sqref="C8:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,179 +668,175 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="C2" s="3"/>
       <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>20</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E2" s="4"/>
       <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="3"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="2"/>
+      <c r="A5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="2"/>
+      <c r="C6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="4"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
+      <c r="A8" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="2" t="s">
-        <v>19</v>
+      <c r="D8" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="D9" s="11"/>
       <c r="E9" s="4"/>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="10"/>
+      <c r="C10" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="4"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="8"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="4"/>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="2" t="s">
-        <v>3</v>
+      <c r="A13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2"/>
+      <c r="B14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="4"/>
       <c r="F14" s="2"/>
     </row>
@@ -783,28 +848,17 @@
       <c r="E15" s="4"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="2"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:F11" xr:uid="{F689A68A-4E99-4027-9313-5972ED85C8C1}"/>
-  <mergeCells count="3">
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
+  <autoFilter ref="A1:F10" xr:uid="{F689A68A-4E99-4027-9313-5972ED85C8C1}"/>
+  <mergeCells count="8">
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D10:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>